<commit_message>
syncronizing github files with desktop
</commit_message>
<xml_diff>
--- a/T2DM iHMP Data/subject data/Subject data T2DM iHMP 5.xlsx
+++ b/T2DM iHMP Data/subject data/Subject data T2DM iHMP 5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\Sabrina_BMS_Bachelor-Internship\T2DM iHMP Data\subject data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729B9D01-011B-4502-AC14-231CD690B4DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AC852A-3BD5-4A6D-836E-1423BD4E1C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -389,6 +389,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -673,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1166,7 +1169,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B61" s="2" t="s">

</xml_diff>

<commit_message>
Update Subject data T2DM iHMP 5.xlsx
</commit_message>
<xml_diff>
--- a/T2DM iHMP Data/subject data/Subject data T2DM iHMP 5.xlsx
+++ b/T2DM iHMP Data/subject data/Subject data T2DM iHMP 5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\Sabrina_BMS_Bachelor-Internship\T2DM iHMP Data\subject data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34420f5773a88cdb/Documents/UM documents/BMS Year 3/Internship ^M Thesis/Sabrina_BMS_Bachelor-Internship/T2DM iHMP Data/subject data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AC852A-3BD5-4A6D-836E-1423BD4E1C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B6AC852A-3BD5-4A6D-836E-1423BD4E1C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4AC82671-67FB-4817-A87D-19D4B5555999}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="50" windowWidth="19200" windowHeight="10150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -385,13 +385,13 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -705,40 +705,40 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -746,39 +746,39 @@
     </row>
     <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>5</v>
+      <c r="A9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
+      <c r="A10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>5</v>
+      <c r="A11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -786,31 +786,31 @@
     </row>
     <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
+      <c r="A14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>5</v>
+      <c r="A15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>3</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="17" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>3</v>
@@ -826,159 +826,159 @@
     </row>
     <row r="18" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
+      <c r="A19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>5</v>
+      <c r="A20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>5</v>
+      <c r="A22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>5</v>
+      <c r="A23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>5</v>
+      <c r="A24" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>5</v>
+      <c r="A26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>5</v>
+      <c r="A27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>5</v>
+      <c r="A28" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>5</v>
+      <c r="A30" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>5</v>
+      <c r="A31" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
-        <v>35</v>
+      <c r="A33" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>3</v>
+      <c r="A34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>3</v>
+      <c r="A36" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>5</v>
@@ -986,95 +986,95 @@
     </row>
     <row r="38" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>3</v>
+      <c r="A39" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>3</v>
+      <c r="A40" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>3</v>
+      <c r="A41" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>3</v>
+      <c r="A43" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>3</v>
+      <c r="A45" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>3</v>
+      <c r="A46" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>3</v>
+      <c r="A48" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>5</v>
@@ -1082,63 +1082,63 @@
     </row>
     <row r="50" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>3</v>
+      <c r="A51" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>3</v>
+      <c r="A52" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>3</v>
+      <c r="A53" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>3</v>
+      <c r="A54" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>3</v>
+      <c r="A55" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>3</v>
+      <c r="A56" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>5</v>
@@ -1146,39 +1146,39 @@
     </row>
     <row r="58" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A61" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>3</v>
+      <c r="B61" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B61">
-    <sortCondition ref="A1"/>
+    <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>